<commit_message>
Simpan perubahan lokal sebelum pull
</commit_message>
<xml_diff>
--- a/Riwayat_Transaksi.xlsx
+++ b/Riwayat_Transaksi.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,257 +436,406 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>No Transaksi</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Nama Barang</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Jumlah</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Tanggal</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Pensil Mekanik</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>8000</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2024-12-05 23:19:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Jangka</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>12000</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2024-12-05 23:19:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Kertas HVS</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2500</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2024-12-05 23:20:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>Penghapus</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2024-12-05 23:20:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
         <v>2</v>
       </c>
-      <c r="C2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2024-11-20 08:32:28</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Pulpen</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="n">
-        <v>3000</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2024-11-20 08:32:37</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Kaos</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Penggaris</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4500</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2024-12-05 23:20:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Isi Binder A4</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>9</v>
+      </c>
+      <c r="D7" t="n">
+        <v>90000</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2024-12-06 10:09:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Es</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>10</v>
+      </c>
+      <c r="D8" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2024-12-06 10:45:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>4</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Cutter</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" t="n">
+        <v>45000</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2024-12-06 10:45:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>4</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Binder A4</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="n">
+        <v>25000</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2024-12-06 10:45:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>5</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Buku Tulis</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2024-12-07 00:15:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>6</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Buku Tulis</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
         <v>2</v>
       </c>
-      <c r="C4" t="n">
-        <v>20000</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2024-11-20 15:42:28</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Pulpen</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
+      <c r="D12" t="n">
+        <v>10000</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2024-12-08 17:46:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>7</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Gunting</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="n">
+        <v>12000</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2024-12-08 22:37:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>8</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Higlighter</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>7000</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2024-12-10 18:51:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>9</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Jangka</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="n">
+        <v>12000</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2024-12-11 09:16:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>10</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Binder A4</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
         <v>2</v>
       </c>
-      <c r="C5" t="n">
-        <v>6000</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2024-11-20 15:42:37</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Pensil</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" t="n">
-        <v>4000</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2024-11-20 15:42:44</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Jangka</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C7" t="n">
-        <v>24000</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>45616.75446518519</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Jangka</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="n">
-        <v>12000</v>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>45616.75975229167</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Pensil</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="n">
-        <v>2000</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>45616.75975231481</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Binder B5</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" t="n">
-        <v>30000</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>45616.79043575231</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="D16" t="n">
+        <v>50000</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2024-12-11 15:36:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>11</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Kalkulator</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" t="n">
+        <v>18000</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2024-12-11 16:13:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>11</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Binder A4</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>3</v>
+      </c>
+      <c r="D18" t="n">
+        <v>75000</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2024-12-11 16:13:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>12</v>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>Brush Pen</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" t="n">
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="n">
         <v>23000</v>
       </c>
-      <c r="D11" s="2" t="n">
-        <v>45616.79256298611</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Kaos</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>2</v>
-      </c>
-      <c r="C12" t="n">
-        <v>20000</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>45616.79676871315</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Brush Pen</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" t="n">
-        <v>23000</v>
-      </c>
-      <c r="D13" s="2" t="n">
-        <v>45616.79676874147</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Kertas HVS</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>2</v>
-      </c>
-      <c r="C14" t="n">
-        <v>500</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>45616.79676876352</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Kertas Folio</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" t="n">
-        <v>500</v>
-      </c>
-      <c r="D15" s="2" t="n">
-        <v>45616.79676877892</v>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2024-12-13 11:56:34</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>